<commit_message>
update plant sampling ID
</commit_message>
<xml_diff>
--- a/templates/dataplant/Plant_sampling.xlsx
+++ b/templates/dataplant/Plant_sampling.xlsx
@@ -1,11 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F0F5FE-B16D-44D7-A3C1-4A47E5D0D3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="isa_template" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="plant_sampling" state="visible" r:id="rId5"/>
+    <sheet name="isa_template" sheetId="1" r:id="rId1"/>
+    <sheet name="plant_sampling" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -20,9 +24,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>f12e98ee-a4e7-4ada-ba56-1e13cce1a44b</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -363,19 +364,22 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/PO_0009046</t>
+  </si>
+  <si>
+    <t>2c588520-2675-444b-87dc-82f3fca431f9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -402,7 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -418,8 +422,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:BB7" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:BB7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="annotationTable" displayName="annotationTable" ref="A1:BB7">
+  <autoFilter ref="A1:BB7" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -476,60 +480,60 @@
     <filterColumn colId="53" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="54">
-    <tableColumn id="1" name="Input [Source Name]" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Protocol Type" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Term Source REF (DPBO:1000161)" totalsRowFunction="none"/>
-    <tableColumn id="4" name="Term Accession Number (DPBO:1000161)" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Protocol REF" totalsRowFunction="none"/>
-    <tableColumn id="6" name="Characteristic [organism]" totalsRowFunction="none"/>
-    <tableColumn id="7" name="Term Source REF (OBI:0100026)" totalsRowFunction="none"/>
-    <tableColumn id="8" name="Term Accession Number (OBI:0100026)" totalsRowFunction="none"/>
-    <tableColumn id="9" name="Characteristic [genotype]" totalsRowFunction="none"/>
-    <tableColumn id="10" name="Term Source REF (EFO:0000513)" totalsRowFunction="none"/>
-    <tableColumn id="11" name="Term Accession Number (EFO:0000513)" totalsRowFunction="none"/>
-    <tableColumn id="12" name="Characteristic [biological replicate]" totalsRowFunction="none"/>
-    <tableColumn id="13" name="Term Source REF (DPBO:0000042)" totalsRowFunction="none"/>
-    <tableColumn id="14" name="Term Accession Number (DPBO:0000042)" totalsRowFunction="none"/>
-    <tableColumn id="15" name="Characteristic [organism part]" totalsRowFunction="none"/>
-    <tableColumn id="16" name="Term Source REF (EFO:0000635)" totalsRowFunction="none"/>
-    <tableColumn id="17" name="Term Accession Number (EFO:0000635)" totalsRowFunction="none"/>
-    <tableColumn id="18" name="Characteristic [plant age]" totalsRowFunction="none"/>
-    <tableColumn id="19" name="Term Source REF (DPBO:0000033)" totalsRowFunction="none"/>
-    <tableColumn id="20" name="Term Accession Number (DPBO:0000033)" totalsRowFunction="none"/>
-    <tableColumn id="21" name="Characteristic [developmental stage]" totalsRowFunction="none"/>
-    <tableColumn id="22" name="Term Source REF (NCIT:C43531)" totalsRowFunction="none"/>
-    <tableColumn id="23" name="Term Accession Number (NCIT:C43531)" totalsRowFunction="none"/>
-    <tableColumn id="24" name="Characteristic [whole plant size]" totalsRowFunction="none"/>
-    <tableColumn id="25" name="Term Source REF (TO:1000012)" totalsRowFunction="none"/>
-    <tableColumn id="26" name="Term Accession Number (TO:1000012)" totalsRowFunction="none"/>
-    <tableColumn id="27" name="Characteristic [phenotype]" totalsRowFunction="none"/>
-    <tableColumn id="28" name="Term Source REF (DPBO:0000073)" totalsRowFunction="none"/>
-    <tableColumn id="29" name="Term Accession Number (DPBO:0000073)" totalsRowFunction="none"/>
-    <tableColumn id="30" name="Characteristic [plant disease]" totalsRowFunction="none"/>
-    <tableColumn id="31" name="Term Source REF (PSO:0000013)" totalsRowFunction="none"/>
-    <tableColumn id="32" name="Term Accession Number (PSO:0000013)" totalsRowFunction="none"/>
-    <tableColumn id="33" name="Characteristic [plant disease stage]" totalsRowFunction="none"/>
-    <tableColumn id="34" name="Term Source REF (DPBO:0000072)" totalsRowFunction="none"/>
-    <tableColumn id="35" name="Term Accession Number (DPBO:0000072)" totalsRowFunction="none"/>
-    <tableColumn id="36" name="Parameter [sample collection date]" totalsRowFunction="none"/>
-    <tableColumn id="37" name="Term Source REF (GENEPIO:0001174)" totalsRowFunction="none"/>
-    <tableColumn id="38" name="Term Accession Number (GENEPIO:0001174)" totalsRowFunction="none"/>
-    <tableColumn id="39" name="Parameter [Reference Time Point]" totalsRowFunction="none"/>
-    <tableColumn id="40" name="Term Source REF (NCIT:C82576)" totalsRowFunction="none"/>
-    <tableColumn id="41" name="Term Accession Number (NCIT:C82576)" totalsRowFunction="none"/>
-    <tableColumn id="42" name="Parameter [sample collected by]" totalsRowFunction="none"/>
-    <tableColumn id="43" name="Term Source REF (GENEPIO:0001153)" totalsRowFunction="none"/>
-    <tableColumn id="44" name="Term Accession Number (GENEPIO:0001153)" totalsRowFunction="none"/>
-    <tableColumn id="45" name="Parameter [sample collection method]" totalsRowFunction="none"/>
-    <tableColumn id="46" name="Term Source REF (DPBO:0000009)" totalsRowFunction="none"/>
-    <tableColumn id="47" name="Term Accession Number (DPBO:0000009)" totalsRowFunction="none"/>
-    <tableColumn id="48" name="Parameter [metabolism quenching method]" totalsRowFunction="none"/>
-    <tableColumn id="49" name="Term Source REF (DPBO:0000010)" totalsRowFunction="none"/>
-    <tableColumn id="50" name="Term Accession Number (DPBO:0000010)" totalsRowFunction="none"/>
-    <tableColumn id="51" name="Parameter [sample storage]" totalsRowFunction="none"/>
-    <tableColumn id="52" name="Term Source REF (DPBO:0000011)" totalsRowFunction="none"/>
-    <tableColumn id="53" name="Term Accession Number (DPBO:0000011)" totalsRowFunction="none"/>
-    <tableColumn id="54" name="Output [Sample Name]" totalsRowFunction="none"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Input [Source Name]" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Protocol Type"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Term Source REF (DPBO:1000161)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Term Accession Number (DPBO:1000161)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Protocol REF"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Characteristic [organism]"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Term Source REF (OBI:0100026)"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Term Accession Number (OBI:0100026)"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Characteristic [genotype]"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Term Source REF (EFO:0000513)"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Term Accession Number (EFO:0000513)"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Characteristic [biological replicate]"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Term Source REF (DPBO:0000042)"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Term Accession Number (DPBO:0000042)"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Characteristic [organism part]"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Term Source REF (EFO:0000635)"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Term Accession Number (EFO:0000635)"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Characteristic [plant age]"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Term Source REF (DPBO:0000033)"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Term Accession Number (DPBO:0000033)"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Characteristic [developmental stage]"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Term Source REF (NCIT:C43531)"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Term Accession Number (NCIT:C43531)"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Characteristic [whole plant size]"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Term Source REF (TO:1000012)"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Term Accession Number (TO:1000012)"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Characteristic [phenotype]"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Term Source REF (DPBO:0000073)"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Term Accession Number (DPBO:0000073)"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Characteristic [plant disease]"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Term Source REF (PSO:0000013)"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Term Accession Number (PSO:0000013)"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Characteristic [plant disease stage]"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Term Source REF (DPBO:0000072)"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Term Accession Number (DPBO:0000072)"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Parameter [sample collection date]"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Term Source REF (GENEPIO:0001174)"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Term Accession Number (GENEPIO:0001174)"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Parameter [Reference Time Point]"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Term Source REF (NCIT:C82576)"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Term Accession Number (NCIT:C82576)"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Parameter [sample collected by]"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Term Source REF (GENEPIO:0001153)"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Term Accession Number (GENEPIO:0001153)"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="Parameter [sample collection method]"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="Term Source REF (DPBO:0000009)"/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="Term Accession Number (DPBO:0000009)"/>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="Parameter [metabolism quenching method]"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="Term Source REF (DPBO:0000010)"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="Term Accession Number (DPBO:0000010)"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="Parameter [sample storage]"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="Term Source REF (DPBO:0000011)"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="Term Accession Number (DPBO:0000011)"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="Output [Sample Name]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -831,1379 +835,1387 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>28</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>29</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>30</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>31</v>
       </c>
-      <c r="G17" t="s">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>33</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>34</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>35</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>36</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>37</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>38</v>
       </c>
-      <c r="G18" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="G20" t="s">
         <v>41</v>
       </c>
-      <c r="G20" t="s">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="G24" t="s">
         <v>46</v>
       </c>
-      <c r="G24" t="s">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BB7"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>58</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>59</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>60</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>61</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>62</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>63</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>64</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>65</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>67</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>68</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>69</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>70</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>71</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>72</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>73</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>74</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>75</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>78</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>79</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>80</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>81</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>82</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>83</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>84</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>85</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>86</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>87</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>88</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>89</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>90</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>91</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>92</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>93</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>94</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>95</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>96</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>97</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>98</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>99</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>100</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>101</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>102</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>103</v>
       </c>
-      <c r="BB1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
         <v>105</v>
       </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>106</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" t="s">
+        <v>104</v>
+      </c>
+      <c r="N2" t="s">
+        <v>104</v>
+      </c>
+      <c r="O2" t="s">
         <v>107</v>
       </c>
-      <c r="H2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K2" t="s">
-        <v>105</v>
-      </c>
-      <c r="L2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M2" t="s">
-        <v>105</v>
-      </c>
-      <c r="N2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>108</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>109</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
+        <v>104</v>
+      </c>
+      <c r="S2" t="s">
+        <v>104</v>
+      </c>
+      <c r="T2" t="s">
+        <v>104</v>
+      </c>
+      <c r="U2" t="s">
+        <v>104</v>
+      </c>
+      <c r="V2" t="s">
+        <v>104</v>
+      </c>
+      <c r="W2" t="s">
+        <v>104</v>
+      </c>
+      <c r="X2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" t="s">
         <v>110</v>
       </c>
-      <c r="R2" t="s">
-        <v>105</v>
-      </c>
-      <c r="S2" t="s">
-        <v>105</v>
-      </c>
-      <c r="T2" t="s">
-        <v>105</v>
-      </c>
-      <c r="U2" t="s">
-        <v>105</v>
-      </c>
-      <c r="V2" t="s">
-        <v>105</v>
-      </c>
-      <c r="W2" t="s">
-        <v>105</v>
-      </c>
-      <c r="X2" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>105</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>105</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O3" t="s">
         <v>111</v>
       </c>
-      <c r="G3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I3" t="s">
-        <v>105</v>
-      </c>
-      <c r="J3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K3" t="s">
-        <v>105</v>
-      </c>
-      <c r="L3" t="s">
-        <v>105</v>
-      </c>
-      <c r="M3" t="s">
-        <v>105</v>
-      </c>
-      <c r="N3" t="s">
-        <v>105</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>112</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>113</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
+        <v>104</v>
+      </c>
+      <c r="S3" t="s">
+        <v>104</v>
+      </c>
+      <c r="T3" t="s">
+        <v>104</v>
+      </c>
+      <c r="U3" t="s">
+        <v>104</v>
+      </c>
+      <c r="V3" t="s">
+        <v>104</v>
+      </c>
+      <c r="W3" t="s">
+        <v>104</v>
+      </c>
+      <c r="X3" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>104</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M4" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" t="s">
+        <v>104</v>
+      </c>
+      <c r="O4" t="s">
         <v>114</v>
       </c>
-      <c r="R3" t="s">
-        <v>105</v>
-      </c>
-      <c r="S3" t="s">
-        <v>105</v>
-      </c>
-      <c r="T3" t="s">
-        <v>105</v>
-      </c>
-      <c r="U3" t="s">
-        <v>105</v>
-      </c>
-      <c r="V3" t="s">
-        <v>105</v>
-      </c>
-      <c r="W3" t="s">
-        <v>105</v>
-      </c>
-      <c r="X3" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" t="s">
-        <v>105</v>
-      </c>
-      <c r="H4" t="s">
-        <v>105</v>
-      </c>
-      <c r="I4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J4" t="s">
-        <v>105</v>
-      </c>
-      <c r="K4" t="s">
-        <v>105</v>
-      </c>
-      <c r="L4" t="s">
-        <v>105</v>
-      </c>
-      <c r="M4" t="s">
-        <v>105</v>
-      </c>
-      <c r="N4" t="s">
-        <v>105</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q4" t="s">
         <v>115</v>
       </c>
-      <c r="P4" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>116</v>
-      </c>
       <c r="R4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Z4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AA4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AB4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AC4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AD4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AE4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AF4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AG4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AH4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AI4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AJ4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AK4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AL4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AM4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AN4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AO4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AP4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AQ4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AR4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AS4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AT4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AU4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AV4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AW4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AX4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AY4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AZ4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BA4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BB4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Z5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AA5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AB5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AC5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AD5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AE5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AF5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AG5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AH5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AI5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AJ5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AK5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AL5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AM5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AN5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AO5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AP5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AQ5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AR5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AS5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AT5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AU5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AV5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AW5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AX5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AY5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AZ5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BA5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BB5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Z6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AA6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AB6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AC6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AD6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AE6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AF6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AG6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AH6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AI6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AJ6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AK6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AL6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AM6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AN6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AO6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AP6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AQ6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AR6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AS6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AT6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AU6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AV6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AW6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AX6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AY6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AZ6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BA6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BB6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Z7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AA7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AB7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AC7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AD7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AE7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AF7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AG7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AH7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AI7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AJ7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AK7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AL7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AM7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AN7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AO7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AP7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AQ7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AR7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AS7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AT7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AU7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AV7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AW7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AX7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AY7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AZ7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BA7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BB7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>